<commit_message>
Added other modules in Ruby to selendroid
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/BatteryIndicator_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/BatteryIndicator_JS.xlsx
@@ -101,87 +101,11 @@
 };
 validate3
 {
-validate_Text_Exists=VT200-0251
+validate_Text_Exists=VT200-0255
 };
 validate4
 {
-validate_Screenshot=VT200_0251
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Battery JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0254
-};
-validate4
-{
-validate_Screenshot=VT200_0254_before
-};
-validate5
-{
-validate_Screenshot=VT200_0254_after
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Battery JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0255
-};
-validate4
-{
 validate_Screenshot=VT200_0255
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Battery JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0256
-};
-validate4
-{
-validate_Screenshot=VT200_0256
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Battery JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0257
-};
-validate4
-{
-validate_Screenshot=VT200_0257
 };</t>
   </si>
   <si>
@@ -293,22 +217,6 @@
 validate1;
 link_Click(battery_test_link);
 validate2;
-SelectTestToRun(VT200_0254_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(3);
-TakeScreenshot(VT200_0254_before);
-validate4;
-wait(10);
-TakeScreenshot(VT200_0254_after);
-validate5;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(battery_test_link);
-validate2;
 SelectTestToRun(VT200_0255_string);
 ClickRunTest(runtest_top_xpath);
 validate3;
@@ -316,33 +224,6 @@
 wait(3);
 TakeScreenshot(VT200_0255);
 validate4;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(battery_test_link);
-validate2;
-SelectTestToRun(VT200_0256_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(3);
-TakeScreenshot(VT200_0256);
-validate4;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(3);
-validate1;
-link_Click(battery_test_link);
-validate2;
-SelectTestToRun(VT200_0257_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(3);
-TakeScreenshot(VT200_0257);
-validate4;
-</t>
   </si>
   <si>
     <t xml:space="preserve">wait(3);
@@ -411,6 +292,123 @@
 ClickRunTest(runtest_bottom_xpath);
 wait(3);
 TakeScreenshot(VT200_0262);
+validate4;
+</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(battery_test_link);
+validate2;
+SelectTestToRun(VT200_0254_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(3);
+validate4;
+wait(10);
+validate5;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Battery JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0254
+};
+validate4
+{
+validate_isIconDisplayed=batteryview_xpath,true
+};
+validate5
+{
+validate_isIconDisplayed=batteryview_xpath,false
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Battery JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0251
+};
+validate4
+{
+validate_Screenshot=VT200_0251
+validate_Iconposition=batteryview_xpath,left,20
+validate_Iconposition=batteryview_xpath,top,40
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Battery JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0256
+};
+validate4
+{
+validate_Iconposition=batteryview_xpath,left,40
+};</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(battery_test_link);
+validate2;
+SelectTestToRun(VT200_0256_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(3);
+validate4;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Battery JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0257
+};
+validate4
+{
+validate_Iconposition=batteryview_xpath,top,40
+};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(3);
+validate1;
+link_Click(battery_test_link);
+validate2;
+SelectTestToRun(VT200_0257_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(3);
 validate4;
 </t>
   </si>
@@ -922,7 +920,7 @@
       </c>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="180.75" thickBot="1">
+    <row r="2" spans="1:11" ht="203.25" thickBot="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -942,10 +940,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>11</v>
@@ -971,10 +969,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -998,10 +996,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1023,10 +1021,10 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1050,10 +1048,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1077,10 +1075,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1104,10 +1102,10 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1131,10 +1129,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1158,10 +1156,10 @@
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1185,10 +1183,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>

</xml_diff>